<commit_message>
Added ability to repace row and column ranges with areas
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaeTypes" sheetId="2" r:id="rId2"/>
+    <sheet name="Ranges" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Hello</t>
   </si>
@@ -41,6 +42,21 @@
   </si>
   <si>
     <t>Arrayed (multiple)</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>This sheet</t>
+  </si>
+  <si>
+    <t>Other sheet</t>
   </si>
 </sst>
 </file>
@@ -89,8 +105,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -99,11 +117,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -576,4 +596,91 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>SUM(F4:F6)</f>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <f>SUM(ValueTypes!A3:A4)</f>
+        <v>4.1415000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>SUM(F:F)</f>
+        <v>6</v>
+      </c>
+      <c r="C3" t="e">
+        <f>SUM(ValueTypes!A:A)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f>SUM(5:5)</f>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>SUM(ValueTypes!4:4)</f>
+        <v>3.1415000000000002</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel_to_ruby now extracts named references
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaeTypes" sheetId="2" r:id="rId2"/>
     <sheet name="Ranges" sheetId="3" r:id="rId3"/>
+    <sheet name="Referencing" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Named_reference">Referencing!$A$1</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Hello</t>
   </si>
@@ -57,6 +61,9 @@
   </si>
   <si>
     <t>Other sheet</t>
+  </si>
+  <si>
+    <t>Named reference</t>
   </si>
 </sst>
 </file>
@@ -602,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -683,4 +690,35 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="str">
+        <f>Named_reference</f>
+        <v>Named reference</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started to add table extraction to the excel_to_ruby_output
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
     <sheet name="FormulaeTypes" sheetId="2" r:id="rId2"/>
     <sheet name="Ranges" sheetId="3" r:id="rId3"/>
     <sheet name="Referencing" sheetId="4" r:id="rId4"/>
+    <sheet name="Tables" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Named_reference">Referencing!$A$1</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Hello</t>
   </si>
@@ -64,6 +65,21 @@
   </si>
   <si>
     <t>Named reference</t>
+  </si>
+  <si>
+    <t>ColA</t>
+  </si>
+  <si>
+    <t>ColB</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -136,6 +152,17 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FirstTable" displayName="FirstTable" ref="B2:C5" totalsRowCount="1">
+  <autoFilter ref="B2:C4"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="ColA" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="ColB" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -721,4 +748,60 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <f>SUBTOTAL(103,FirstTable[ColB])</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ruby_to_excel.rb now allows values that should be changable at runtime to be specified
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -744,23 +744,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="str">
         <f>Named_reference</f>
         <v>Named reference</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f>A4+1</f>
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <f>B4+1</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the example excel model a bit, and implemented the match and join functions
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -128,8 +128,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -146,19 +150,23 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -181,7 +189,7 @@
       <totalsRowFormula>SUM(FirstTable[ColB])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" name="Column1" dataDxfId="0">
-      <calculatedColumnFormula>FirstTable[[#This Row],[ColA]:[ColB]]</calculatedColumnFormula>
+      <calculatedColumnFormula>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -513,7 +521,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -788,10 +796,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -806,10 +814,6 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="e">
-        <f>FirstTable[[#Headers],[ColB]:[Column1]]</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="3" spans="2:8">
       <c r="B3">
@@ -818,9 +822,9 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="e">
-        <f>FirstTable[[#This Row],[ColA]:[ColB]]</f>
-        <v>#VALUE!</v>
+      <c r="D3" t="str">
+        <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
+        <v>1A</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -830,21 +834,21 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="e">
-        <f>FirstTable[[#This Row],[ColA]:[ColB]]</f>
-        <v>#VALUE!</v>
+      <c r="D4" t="str">
+        <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
+        <v>2B</v>
       </c>
       <c r="F4" t="str">
         <f>FirstTable[[#This Row],[ColB]]</f>
         <v>B</v>
       </c>
-      <c r="G4" t="e">
-        <f>FirstTable[#This Row]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H4" t="e">
-        <f>FirstTable[[#This Row],[ColB]:[Column1]]</f>
-        <v>#VALUE!</v>
+      <c r="G4">
+        <f>MATCH("2B",FirstTable[#This Row],FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f>MATCH("B",FirstTable[[#This Row],[ColB]:[Column1]])</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -858,37 +862,65 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="E6" t="e">
-        <f>FirstTable[#Headers]</f>
-        <v>#VALUE!</v>
+      <c r="E6" t="str">
+        <f t="array" ref="E6:G6">FirstTable[#Headers]</f>
+        <v>ColA</v>
+      </c>
+      <c r="F6" t="str">
+        <v>ColB</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Column1</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="E7" t="e">
-        <f>FirstTable[#Totals]</f>
-        <v>#VALUE!</v>
+      <c r="E7">
+        <f t="array" ref="E7:G7">FirstTable[#Totals]</f>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="E8" t="e">
-        <f>FirstTable[#All]</f>
-        <v>#VALUE!</v>
+      <c r="E8" t="str">
+        <f t="array" ref="E8:G11">FirstTable[#All]</f>
+        <v>ColA</v>
+      </c>
+      <c r="F8" t="str">
+        <v>ColB</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Column1</v>
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="E9" t="e">
-        <f>SUM(FirstTable[#Data])</f>
-        <v>#VALUE!</v>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>A</v>
+      </c>
+      <c r="G9" t="str">
+        <v>1A</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="C10">
-        <f>FirstTable[#Totals]</f>
-        <v>0</v>
-      </c>
-      <c r="E10" t="e">
-        <f>SUM(FirstTable[])</f>
-        <v>#VALUE!</v>
+        <f>SUM(FirstTable[#Totals])</f>
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="str">
+        <v>B</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2B</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -896,10 +928,31 @@
         <f>SUM(FirstTable[ColA])</f>
         <v>3</v>
       </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:8">
       <c r="C12">
         <f>FirstTable[[#Totals],[ColA]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="C13">
+        <f>SUM(FirstTable[#Data])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="C14">
+        <f>SUM(FirstTable[])</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simple indirects to simple named references now work
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -782,6 +782,12 @@
       <c r="C4">
         <f>B4+1</f>
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="str">
+        <f ca="1">INDIRECT("naMed_reFerence")</f>
+        <v>Named reference</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Can now replace indirects that contain strings that refer to cells, named references or tables
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -752,7 +752,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -788,6 +788,12 @@
       <c r="B8" t="str">
         <f ca="1">INDIRECT("naMed_reFerence")</f>
         <v>Named reference</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9">
+        <f ca="1">SUM(INDIRECT("firsttable[#Totals]"))</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -805,7 +811,7 @@
   <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added the first step in optimising to excel_to_ruby.rb whereby functions where all the arguments are static values are replaced
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -755,7 +755,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -782,6 +782,12 @@
       <c r="C4">
         <f>B4+1</f>
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <f>1+1+1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
excel_to_ruby now does multiple passes, converting to values then replacing indirects
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Hello</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Named</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -752,26 +758,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="str">
         <f>Named_reference</f>
         <v>Named reference</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>10</v>
       </c>
@@ -784,22 +790,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f>1+1+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="B8" t="str">
         <f ca="1">INDIRECT("naMed_reFerence")</f>
         <v>Named reference</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="B9">
         <f ca="1">SUM(INDIRECT("firsttable[#Totals]"))</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="str">
+        <f ca="1">INDIRECT(B11&amp;"_"&amp;C11)</f>
+        <v>Named reference</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel_to_ruby.rb now has functionality to prune unwanted formulae
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Hello</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Other sheet</t>
-  </si>
-  <si>
-    <t>Named reference</t>
   </si>
   <si>
     <t>ColA</t>
@@ -760,21 +757,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1">
+        <f>C4</f>
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="str">
+      <c r="A2">
         <f>Named_reference</f>
-        <v>Named reference</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -797,9 +795,9 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" t="str">
+      <c r="B8">
         <f ca="1">INDIRECT("naMed_reFerence")</f>
-        <v>Named reference</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -810,14 +808,14 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="str">
+      <c r="D11">
         <f ca="1">INDIRECT(B11&amp;"_"&amp;C11)</f>
-        <v>Named reference</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -832,43 +830,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <f ca="1">Referencing!D11</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="str">
         <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
         <v>1A</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="1:8">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="str">
         <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
@@ -887,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="1:8">
       <c r="B5">
         <f>SUM(FirstTable[ColA])</f>
         <v>3</v>
@@ -897,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="1:8">
       <c r="E6" t="str">
         <f t="array" ref="E6:G6">FirstTable[#Headers]</f>
         <v>ColA</v>
@@ -909,7 +913,7 @@
         <v>Column1</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="1:8">
       <c r="E7">
         <f t="array" ref="E7:G7">FirstTable[#Totals]</f>
         <v>3</v>
@@ -921,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="1:8">
       <c r="E8" t="str">
         <f t="array" ref="E8:G11">FirstTable[#All]</f>
         <v>ColA</v>
@@ -933,7 +937,7 @@
         <v>Column1</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="1:8">
       <c r="E9">
         <v>1</v>
       </c>
@@ -944,7 +948,7 @@
         <v>1A</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="1:8">
       <c r="C10">
         <f>SUM(FirstTable[#Totals])</f>
         <v>3</v>
@@ -959,7 +963,7 @@
         <v>2B</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="1:8">
       <c r="C11">
         <f>SUM(FirstTable[ColA])</f>
         <v>3</v>
@@ -974,19 +978,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="1:8">
       <c r="C12">
         <f>FirstTable[[#Totals],[ColA]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="1:8">
       <c r="C13">
         <f>SUM(FirstTable[#Data])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="1:8">
       <c r="C14">
         <f>SUM(FirstTable[])</f>
         <v>3</v>

</xml_diff>

<commit_message>
Deal with strange characters when generating ruby class names from sheet names
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Ranges" sheetId="3" r:id="rId3"/>
     <sheet name="Referencing" sheetId="4" r:id="rId4"/>
     <sheet name="Tables" sheetId="5" r:id="rId5"/>
+    <sheet name="(innapropriate) sheet name!" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Named_reference">Referencing!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -832,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1008,4 +1009,30 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="3:3">
+      <c r="C4">
+        <f>ValueTypes!A3</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rewrote commands to clean up the filenames in generated intermediate files
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -756,27 +756,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1">
         <f>C4</f>
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2">
         <f>Named_reference</f>
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -789,34 +789,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5">
         <f>1+1+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="B8">
         <f ca="1">INDIRECT("naMed_reFerence")</f>
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="B9">
         <f ca="1">SUM(INDIRECT("firsttable[#Totals]"))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
-      </c>
-      <c r="D11">
-        <f ca="1">INDIRECT(B11&amp;"_"&amp;C11)</f>
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -834,15 +830,15 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1">
-        <f ca="1">Referencing!D11</f>
-        <v>12</v>
+        <f>Referencing!D11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1015,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed the default match_type in the MATCH function to be 1
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>Hello</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Gamma</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
@@ -953,7 +956,7 @@
     <row r="9" spans="1:6">
       <c r="B9">
         <f ca="1">SUM(INDIRECT("firsttable[#Totals]"))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1587,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1613,34 +1616,34 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="str">
         <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
-        <v>1A</v>
+        <v>AA</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="str">
         <f>FirstTable[[#This Row],[ColA]]&amp;FirstTable[[#This Row],[ColB]]</f>
-        <v>2B</v>
+        <v>ZB</v>
       </c>
       <c r="F4" t="str">
         <f>FirstTable[[#This Row],[ColB]]</f>
         <v>B</v>
       </c>
       <c r="G4">
-        <f>MATCH("2B",FirstTable[#This Row],FALSE)</f>
+        <f>MATCH("ZB",FirstTable[#This Row],FALSE)</f>
         <v>3</v>
       </c>
       <c r="H4">
@@ -1651,7 +1654,7 @@
     <row r="5" spans="1:8">
       <c r="B5">
         <f>SUM(FirstTable[ColA])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>SUM(FirstTable[ColB])</f>
@@ -1673,7 +1676,7 @@
     <row r="7" spans="1:8">
       <c r="E7">
         <f t="array" ref="E7:G7">FirstTable[#Totals]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1695,38 +1698,38 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="E9">
-        <v>1</v>
+      <c r="E9" t="str">
+        <v>A</v>
       </c>
       <c r="F9" t="str">
         <v>A</v>
       </c>
       <c r="G9" t="str">
-        <v>1A</v>
+        <v>AA</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="C10">
         <f>SUM(FirstTable[#Totals])</f>
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Z</v>
       </c>
       <c r="F10" t="str">
         <v>B</v>
       </c>
       <c r="G10" t="str">
-        <v>2B</v>
+        <v>ZB</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="C11">
         <f>SUM(FirstTable[ColA])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1738,19 +1741,25 @@
     <row r="12" spans="1:8">
       <c r="C12">
         <f>FirstTable[[#Totals],[ColA]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="C13">
         <f>SUM(FirstTable[#Data])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14">
         <f>SUM(FirstTable[])</f>
-        <v>3</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" t="b">
+        <f>IF(C4&gt;D4,TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>